<commit_message>
feat: change diet composition, more detailed results for diet composition, use of CB153 instead of sumPCB for species scenarios
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PCB_ng_glw/5.BMF_compare_PCB.xlsx
+++ b/inst/results/BMF_computation_PCB_ng_glw/5.BMF_compare_PCB.xlsx
@@ -365,22 +365,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>BMF_species</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>BMF_diet</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>BMF_species</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>BMF_TL_species</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>BMF_TL_diet</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>BMF_TL_species</t>
         </is>
       </c>
     </row>
@@ -392,22 +392,22 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>1.05 [0.77-1.15]</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>1.72 [1.07-2.41]</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>1.05 [0.77-1.15]</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>4.95 [1.23-13.23]</t>
+          <t>1.05 [0.71-1.31]</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1.05 [0.71-1.31]</t>
+          <t>2.33 [0.61-6.39]</t>
         </is>
       </c>
     </row>
@@ -419,22 +419,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>0.63 [0.37-0.93]</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>0.72 [0.38-1.53]</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.63 [0.37-0.93]</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.38 [0.06-3.45]</t>
+          <t>0.48 [0.36-0.77]</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.48 [0.36-0.77]</t>
+          <t>0.26 [0.04-2.03]</t>
         </is>
       </c>
     </row>
@@ -446,22 +446,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>0.3 [0.12-0.72]</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>0.31 [0.11-0.93]</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>0.3 [0.12-0.72]</t>
-        </is>
-      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.03 [0-0.81]</t>
+          <t>0.26 [0.14-0.4]</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.26 [0.14-0.4]</t>
+          <t>0.02 [0-0.5]</t>
         </is>
       </c>
     </row>
@@ -473,22 +473,22 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>0.81 [0.54-1.4]</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>1.34 [0.69-2.44]</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>0.81 [0.54-1.4]</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2.35 [0.34-13.74]</t>
+          <t>0.68 [0.46-1.31]</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.68 [0.46-1.31]</t>
+          <t>1.24 [0.2-7.01]</t>
         </is>
       </c>
     </row>
@@ -500,22 +500,22 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>0.98 [0.54-1.32]</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>1.42 [0.73-2.52]</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>0.98 [0.54-1.32]</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.81 [0.4-15.02]</t>
+          <t>0.82 [0.43-1.29]</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.82 [0.43-1.29]</t>
+          <t>1.58 [0.2-6.91]</t>
         </is>
       </c>
     </row>
@@ -527,22 +527,22 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>1.21 [0.63-1.63]</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>1.77 [0.78-2.66]</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1.21 [0.63-1.63]</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>5.33 [0.49-17.59]</t>
+          <t>1.15 [0.62-1.74]</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1.15 [0.62-1.74]</t>
+          <t>3.13 [0.33-11.23]</t>
         </is>
       </c>
     </row>
@@ -554,22 +554,22 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>1.02 [0.73-1.41]</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>2.05 [1.26-2.94]</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1.02 [0.73-1.41]</t>
-        </is>
-      </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8.19 [1.99-23.73]</t>
+          <t>1.06 [0.72-1.4]</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1.06 [0.72-1.4]</t>
+          <t>2.99 [0.74-8.77]</t>
         </is>
       </c>
     </row>
@@ -581,22 +581,22 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>0.99 [0.66-1.34]</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>1.98 [0.81-3.02]</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0.99 [0.66-1.34]</t>
-        </is>
-      </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>7.39 [0.55-25.55]</t>
+          <t>0.88 [0.58-1.37]</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.88 [0.58-1.37]</t>
+          <t>3.22 [0.31-11.07]</t>
         </is>
       </c>
     </row>
@@ -608,22 +608,22 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>0.89 [0.65-1.19]</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>1.8 [1.15-3.07]</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0.89 [0.65-1.19]</t>
-        </is>
-      </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>5.59 [1.51-26.84]</t>
+          <t>0.83 [0.59-1.1]</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.83 [0.59-1.1]</t>
+          <t>2 [0.54-9.87]</t>
         </is>
       </c>
     </row>
@@ -635,22 +635,22 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>1.16 [0.87-1.52]</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>1.82 [1.09-2.89]</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>1.16 [0.87-1.52]</t>
-        </is>
-      </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>5.8 [1.3-22.55]</t>
+          <t>1.12 [0.8-1.62]</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1.12 [0.8-1.62]</t>
+          <t>3.94 [0.77-12.31]</t>
         </is>
       </c>
     </row>
@@ -662,22 +662,22 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>0.95 [0.72-1.16]</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>2.08 [1.28-2.95]</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0.95 [0.72-1.16]</t>
-        </is>
-      </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>8.63 [2.06-23.89]</t>
+          <t>0.9 [0.62-1.31]</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.9 [0.62-1.31]</t>
+          <t>3.03 [0.75-8.47]</t>
         </is>
       </c>
     </row>
@@ -689,22 +689,22 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>0.68 [0.5-0.89]</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>1.31 [0.86-2.16]</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>0.68 [0.5-0.89]</t>
-        </is>
-      </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2.2 [0.63-9.64]</t>
+          <t>0.54 [0.44-0.7]</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.54 [0.44-0.7]</t>
+          <t>0.79 [0.23-3.52]</t>
         </is>
       </c>
     </row>
@@ -716,22 +716,22 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>1.03 [0.79-1.35]</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>1.75 [1.08-2.98]</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>1.03 [0.79-1.35]</t>
-        </is>
-      </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5.17 [1.24-24.58]</t>
+          <t>1.01 [0.74-1.64]</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1.01 [0.74-1.64]</t>
+          <t>2.64 [0.63-10.42]</t>
         </is>
       </c>
     </row>
@@ -743,22 +743,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>0.77 [0.65-0.98]</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>1.52 [1-2.19]</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>0.77 [0.65-0.98]</t>
-        </is>
-      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3.4 [1-10.04]</t>
+          <t>0.75 [0.61-0.92]</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.75 [0.61-0.92]</t>
+          <t>1.26 [0.37-3.76]</t>
         </is>
       </c>
     </row>
@@ -770,22 +770,22 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>1.1 [0.83-1.28]</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>2.01 [1.24-2.68]</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>1.1 [0.83-1.28]</t>
-        </is>
-      </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>7.78 [1.9-17.97]</t>
+          <t>1.09 [0.78-1.3]</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1.09 [0.78-1.3]</t>
+          <t>3.41 [0.82-7.86]</t>
         </is>
       </c>
     </row>
@@ -797,22 +797,22 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>1.04 [0.72-1.32]</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>1.07 [0.6-1.35]</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>1.04 [0.72-1.32]</t>
-        </is>
-      </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.22 [0.22-2.39]</t>
+          <t>0.97 [0.68-1.16]</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.97 [0.68-1.16]</t>
+          <t>1.29 [0.23-2.69]</t>
         </is>
       </c>
     </row>
@@ -824,22 +824,22 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>1.11 [0.72-1.64]</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>1.35 [0.77-2.22]</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>1.11 [0.72-1.64]</t>
-        </is>
-      </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2.43 [0.46-10.42]</t>
+          <t>0.83 [0.64-1.58]</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.83 [0.64-1.58]</t>
+          <t>1.45 [0.35-6.49]</t>
         </is>
       </c>
     </row>
@@ -851,22 +851,22 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>1.16 [0.75-1.71]</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>1.76 [0.73-2.77]</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>1.16 [0.75-1.71]</t>
-        </is>
-      </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>5.28 [0.39-19.85]</t>
+          <t>1.1 [0.65-1.36]</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1.1 [0.65-1.36]</t>
+          <t>2.55 [0.34-9.75]</t>
         </is>
       </c>
     </row>
@@ -878,22 +878,22 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>0.93 [0.73-1.02]</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>1.6 [0.68-2.53]</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>0.93 [0.73-1.02]</t>
-        </is>
-      </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3.97 [0.33-15.24]</t>
+          <t>0.84 [0.66-0.94]</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.84 [0.66-0.94]</t>
+          <t>1.9 [0.29-7.15]</t>
         </is>
       </c>
     </row>
@@ -905,22 +905,22 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>0.77 [0.57-1.14]</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>1.08 [0.68-1.94]</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>0.77 [0.57-1.14]</t>
-        </is>
-      </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.24 [0.33-6.98]</t>
+          <t>0.66 [0.5-1.14]</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.66 [0.5-1.14]</t>
+          <t>0.73 [0.23-3.93]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
on refait scenario TL diet not ok
</commit_message>
<xml_diff>
--- a/inst/results/BMF_computation_PCB_ng_glw/5.BMF_compare_PCB.xlsx
+++ b/inst/results/BMF_computation_PCB_ng_glw/5.BMF_compare_PCB.xlsx
@@ -407,7 +407,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2.33 [0.61-6.39]</t>
+          <t>4.94 [1.23-13.22]</t>
         </is>
       </c>
     </row>
@@ -434,7 +434,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.26 [0.04-2.03]</t>
+          <t>0.38 [0.06-3.45]</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.02 [0-0.5]</t>
+          <t>0.03 [0-0.81]</t>
         </is>
       </c>
     </row>
@@ -488,7 +488,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1.24 [0.2-7.01]</t>
+          <t>2.35 [0.34-13.73]</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1.58 [0.2-6.91]</t>
+          <t>2.81 [0.4-15.01]</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3.13 [0.33-11.23]</t>
+          <t>5.33 [0.49-17.58]</t>
         </is>
       </c>
     </row>
@@ -569,7 +569,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2.99 [0.74-8.77]</t>
+          <t>8.18 [1.99-23.7]</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>3.22 [0.31-11.07]</t>
+          <t>7.38 [0.55-25.52]</t>
         </is>
       </c>
     </row>
@@ -623,7 +623,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2 [0.54-9.87]</t>
+          <t>5.59 [1.5-26.81]</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3.94 [0.77-12.31]</t>
+          <t>5.8 [1.3-22.53]</t>
         </is>
       </c>
     </row>
@@ -677,7 +677,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>3.03 [0.75-8.47]</t>
+          <t>8.62 [2.06-23.86]</t>
         </is>
       </c>
     </row>
@@ -704,7 +704,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.79 [0.23-3.52]</t>
+          <t>2.2 [0.63-9.63]</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2.64 [0.63-10.42]</t>
+          <t>5.17 [1.24-24.56]</t>
         </is>
       </c>
     </row>
@@ -758,7 +758,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1.26 [0.37-3.76]</t>
+          <t>3.39 [1-10.03]</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3.41 [0.82-7.86]</t>
+          <t>7.78 [1.9-17.95]</t>
         </is>
       </c>
     </row>
@@ -812,7 +812,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1.29 [0.23-2.69]</t>
+          <t>1.22 [0.22-2.39]</t>
         </is>
       </c>
     </row>
@@ -839,7 +839,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1.45 [0.35-6.49]</t>
+          <t>2.43 [0.46-10.41]</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2.55 [0.34-9.75]</t>
+          <t>5.27 [0.39-19.83]</t>
         </is>
       </c>
     </row>
@@ -893,7 +893,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1.9 [0.29-7.15]</t>
+          <t>3.97 [0.33-15.23]</t>
         </is>
       </c>
     </row>
@@ -920,7 +920,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.73 [0.23-3.93]</t>
+          <t>1.24 [0.33-6.98]</t>
         </is>
       </c>
     </row>

</xml_diff>